<commit_message>
Code seems to work again
- Testing required
- Scenarios need to be added
- Discussion on costs
</commit_message>
<xml_diff>
--- a/Data/transport_costs_emissions_raw.xlsx
+++ b/Data/transport_costs_emissions_raw.xlsx
@@ -8,26 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E757EC-51D5-4055-A083-D4CEA2E25D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{F2E757EC-51D5-4055-A083-D4CEA2E25D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D63163B-1410-4368-9739-9E7E269DD291}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="28800" windowHeight="23400" firstSheet="2" activeTab="8" xr2:uid="{5AE32870-AF16-462E-B631-817A89F76936}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="28800" windowHeight="23400" xr2:uid="{5AE32870-AF16-462E-B631-817A89F76936}"/>
   </bookViews>
   <sheets>
-    <sheet name="Costs_OLD" sheetId="1" r:id="rId1"/>
-    <sheet name="base_emissions" sheetId="23" r:id="rId2"/>
-    <sheet name="rel_emission_factors" sheetId="24" r:id="rId3"/>
-    <sheet name="transfer_costs" sheetId="9" r:id="rId4"/>
-    <sheet name="raw_data" sheetId="10" r:id="rId5"/>
-    <sheet name="base_costs_intermediate" sheetId="11" r:id="rId6"/>
-    <sheet name="base_costs" sheetId="17" r:id="rId7"/>
-    <sheet name="EUR_TO_NOK" sheetId="20" r:id="rId8"/>
-    <sheet name="prod_to_vehicle" sheetId="19" r:id="rId9"/>
-    <sheet name="vehicle_cap" sheetId="15" r:id="rId10"/>
-    <sheet name="cost_factors" sheetId="16" r:id="rId11"/>
-    <sheet name="CO2_fee" sheetId="25" r:id="rId12"/>
-    <sheet name="assumptions" sheetId="12" r:id="rId13"/>
-    <sheet name="Sources costs" sheetId="21" r:id="rId14"/>
-    <sheet name="Sources emissions" sheetId="22" r:id="rId15"/>
+    <sheet name="LEGEND" sheetId="27" r:id="rId1"/>
+    <sheet name="Costs_OLD" sheetId="1" r:id="rId2"/>
+    <sheet name="base_emissions" sheetId="23" r:id="rId3"/>
+    <sheet name="rel_emission_factors" sheetId="24" r:id="rId4"/>
+    <sheet name="transfer_costs" sheetId="9" r:id="rId5"/>
+    <sheet name="raw_data" sheetId="10" r:id="rId6"/>
+    <sheet name="base_costs_intermediate" sheetId="11" r:id="rId7"/>
+    <sheet name="base_costs" sheetId="17" r:id="rId8"/>
+    <sheet name="EUR_TO_NOK" sheetId="20" r:id="rId9"/>
+    <sheet name="prod_to_vehicle" sheetId="19" r:id="rId10"/>
+    <sheet name="lifetimes" sheetId="26" r:id="rId11"/>
+    <sheet name="vehicle_cap" sheetId="15" r:id="rId12"/>
+    <sheet name="cost_factors" sheetId="16" r:id="rId13"/>
+    <sheet name="CO2_fee" sheetId="25" r:id="rId14"/>
+    <sheet name="assumptions" sheetId="12" r:id="rId15"/>
+    <sheet name="Sources costs" sheetId="21" r:id="rId16"/>
+    <sheet name="Sources emissions" sheetId="22" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3324" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="240">
   <si>
     <t>Mode</t>
   </si>
@@ -751,6 +753,60 @@
   <si>
     <t>Biodiesel timber trains: in original excel file, they used a relative cost factor w.r.t. diesel of 0.3 instead of 0.2 (only for timber). I used 0.2 for all product groups</t>
   </si>
+  <si>
+    <t>Lifetime</t>
+  </si>
+  <si>
+    <t>base_emissions</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>rel_emissions_factors</t>
+  </si>
+  <si>
+    <t>transfer_costs</t>
+  </si>
+  <si>
+    <t>raw_data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_costs  </t>
+  </si>
+  <si>
+    <t>base_costs_intermediate</t>
+  </si>
+  <si>
+    <t>EUR_TO_NOK</t>
+  </si>
+  <si>
+    <t>prod_to_vehicle</t>
+  </si>
+  <si>
+    <t>lifetimes</t>
+  </si>
+  <si>
+    <t>vehicle_cap</t>
+  </si>
+  <si>
+    <t>cost_factors</t>
+  </si>
+  <si>
+    <t>CO2_fee</t>
+  </si>
+  <si>
+    <t>assumptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'sources emissions'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'sources costs'</t>
+  </si>
 </sst>
 </file>
 
@@ -1006,7 +1062,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1044,6 +1100,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1362,6 +1419,1969 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C55ED1A2-26F7-4BE8-B03B-AC0D518020AD}">
+  <dimension ref="B1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="37" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="37" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" location="base_emissions!A1" display="base_emissions" xr:uid="{47E66D54-AD55-441F-A720-671D02BE1428}"/>
+    <hyperlink ref="B3" location="rel_emission_factors!A1" display="rel_emissions_factors" xr:uid="{C4F3C6FE-71EE-4A2F-B080-47BAD5A54787}"/>
+    <hyperlink ref="B4" location="transfer_costs!A1" display="transfer_costs" xr:uid="{18B54721-1CA7-4A52-9407-C984DCE86D06}"/>
+    <hyperlink ref="B5" location="raw_data!A1" display="raw_data" xr:uid="{8CB353DF-A464-458F-890B-D26BCFB29666}"/>
+    <hyperlink ref="B6" location="base_costs_intermediate!A1" display="base_costs_intermediate" xr:uid="{DAE79DE1-E819-4229-A7BA-027D53BCD791}"/>
+    <hyperlink ref="B7" location="base_costs!A1" display="base_costs  " xr:uid="{67E9AD3D-7015-4EC5-9FB4-9E780BC525AE}"/>
+    <hyperlink ref="B8" location="EUR_TO_NOK!A1" display="EUR_TO_NOK" xr:uid="{1D4A29C0-5D69-42EE-986C-B50C1111AFC3}"/>
+    <hyperlink ref="B9" location="prod_to_vehicle!A1" display="prod_to_veh" xr:uid="{6A9754FF-6739-4060-AAF8-E90160D55C9C}"/>
+    <hyperlink ref="B10" location="lifetimes!A1" display="lifetimes" xr:uid="{83FEC15E-890B-4FEA-94A1-29FCD7275831}"/>
+    <hyperlink ref="B11" location="vehicle_cap!A1" display="vehicle_cap" xr:uid="{AA225BC6-6A24-465A-AC1D-F554FA3414EE}"/>
+    <hyperlink ref="B12" location="cost_factors!A1" display="cost_factors" xr:uid="{204D38F5-F7F8-42D9-9983-7B4DF8472CD3}"/>
+    <hyperlink ref="B13" location="CO2_fee!A1" display="CO2_fee" xr:uid="{F9B55AFB-090A-44E4-9AE4-16413FF7D6D1}"/>
+    <hyperlink ref="B14" location="assumptions!A1" display="assumptions" xr:uid="{B6E585B8-9E98-4662-897D-CD0E8A1C362D}"/>
+    <hyperlink ref="B15" location="'Sources costs'!A1" display=" 'sources costs'" xr:uid="{F51D5ECD-C5D0-40EA-9688-2EC4076EA13A}"/>
+    <hyperlink ref="B16" location="'Sources emissions'!A1" display=" 'sources emissions'" xr:uid="{F588768E-EB75-412F-8F3C-75163592EA54}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4663A21-150A-4914-BC6D-954E6813A5C4}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9569D7EE-B770-468F-B61A-E0DB82253C9A}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61F1785-A9D2-43D6-AF64-887423AF0701}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>8500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87DB01C-C28B-4466-B068-FD0A64E87CCA}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D2" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2020</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2025</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2030</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2040</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2050</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>1.3</v>
+      </c>
+      <c r="E5">
+        <v>1.03</v>
+      </c>
+      <c r="F5">
+        <v>0.91</v>
+      </c>
+      <c r="G5">
+        <v>0.85</v>
+      </c>
+      <c r="H5">
+        <v>0.83</v>
+      </c>
+      <c r="J5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>1.06</v>
+      </c>
+      <c r="E7">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F7">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="G7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="H7">
+        <v>1.17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E8">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="F8">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G8">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="H8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H10">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>1.07</v>
+      </c>
+      <c r="E11">
+        <v>1.07</v>
+      </c>
+      <c r="F11">
+        <v>1.07</v>
+      </c>
+      <c r="G11">
+        <v>1.07</v>
+      </c>
+      <c r="H11">
+        <v>1.07</v>
+      </c>
+      <c r="J11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>1.2</v>
+      </c>
+      <c r="E14">
+        <v>1.22</v>
+      </c>
+      <c r="F14">
+        <v>1.24</v>
+      </c>
+      <c r="G14">
+        <v>1.26</v>
+      </c>
+      <c r="H14">
+        <v>1.28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15">
+        <v>1.05</v>
+      </c>
+      <c r="E15">
+        <v>1.05</v>
+      </c>
+      <c r="F15">
+        <v>1.05</v>
+      </c>
+      <c r="G15">
+        <v>1.05</v>
+      </c>
+      <c r="H15">
+        <v>1.05</v>
+      </c>
+      <c r="I15" t="s">
+        <v>141</v>
+      </c>
+      <c r="J15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>1.2</v>
+      </c>
+      <c r="E16">
+        <v>1.2</v>
+      </c>
+      <c r="F16">
+        <v>1.2</v>
+      </c>
+      <c r="G16">
+        <v>1.2</v>
+      </c>
+      <c r="H16">
+        <v>1.2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H18">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>1.2</v>
+      </c>
+      <c r="E19">
+        <v>1.18</v>
+      </c>
+      <c r="F19">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="G19">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="H19">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>1.8</v>
+      </c>
+      <c r="F20">
+        <v>1.6</v>
+      </c>
+      <c r="G20">
+        <v>1.4</v>
+      </c>
+      <c r="H20">
+        <v>1.25</v>
+      </c>
+      <c r="J20" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <v>1.05</v>
+      </c>
+      <c r="E21">
+        <v>1.06</v>
+      </c>
+      <c r="F21">
+        <v>1.07</v>
+      </c>
+      <c r="G21">
+        <v>1.08</v>
+      </c>
+      <c r="H21">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="J21" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A26ADBE-5182-4739-A39F-809BE890F4A3}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2" s="8">
+        <v>5.44E-4</v>
+      </c>
+      <c r="C2" s="8">
+        <v>5.44E-4</v>
+      </c>
+      <c r="D2" s="8">
+        <v>5.44E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2025</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1.2720000000000001E-3</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.7719999999999999E-3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>5.44E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2030</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>5.44E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2040</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3.4559999999999999E-3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>5.4559999999999999E-3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>5.44E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2050</v>
+      </c>
+      <c r="B6" s="8">
+        <v>4.9120000000000006E-3</v>
+      </c>
+      <c r="C6" s="8">
+        <v>7.9119999999999989E-3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>5.44E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BE84BF-E76A-402B-AF31-6F26AF2044C4}">
+  <dimension ref="A1:A22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="144.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96CB461-6F71-44E3-A168-71729D7C3877}">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="116.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>185</v>
+      </c>
+      <c r="B15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A21" r:id="rId1" xr:uid="{6BB6211E-19A0-4F02-BC7A-3A56508CA64B}"/>
+    <hyperlink ref="A19" r:id="rId2" xr:uid="{E125BC90-7F30-4B94-A86A-3EFCF7E2E423}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD9D518-1F19-4A80-A28B-711CA74E3278}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="116.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="35" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>209</v>
+      </c>
+      <c r="B14" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A14" r:id="rId1" xr:uid="{C4319978-B66A-4039-B91C-E1EE64F3642A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA46F70C-1634-4B80-BD59-B77731E4E671}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R631"/>
@@ -28095,1366 +30115,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61F1785-A9D2-43D6-AF64-887423AF0701}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8">
-        <v>8500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87DB01C-C28B-4466-B068-FD0A64E87CCA}">
-  <dimension ref="A1:J21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="45.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D2" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2020</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2025</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2030</v>
-      </c>
-      <c r="G3" s="1">
-        <v>2040</v>
-      </c>
-      <c r="H3" s="1">
-        <v>2050</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>1.3</v>
-      </c>
-      <c r="E5">
-        <v>1.03</v>
-      </c>
-      <c r="F5">
-        <v>0.91</v>
-      </c>
-      <c r="G5">
-        <v>0.85</v>
-      </c>
-      <c r="H5">
-        <v>0.83</v>
-      </c>
-      <c r="J5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7">
-        <v>1.06</v>
-      </c>
-      <c r="E7">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="F7">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="G7">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="H7">
-        <v>1.17</v>
-      </c>
-      <c r="I7" t="s">
-        <v>141</v>
-      </c>
-      <c r="J7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="E8">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="F8">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="G8">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="H8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I8" t="s">
-        <v>141</v>
-      </c>
-      <c r="J8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H10">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11">
-        <v>1.07</v>
-      </c>
-      <c r="E11">
-        <v>1.07</v>
-      </c>
-      <c r="F11">
-        <v>1.07</v>
-      </c>
-      <c r="G11">
-        <v>1.07</v>
-      </c>
-      <c r="H11">
-        <v>1.07</v>
-      </c>
-      <c r="J11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14">
-        <v>1.2</v>
-      </c>
-      <c r="E14">
-        <v>1.22</v>
-      </c>
-      <c r="F14">
-        <v>1.24</v>
-      </c>
-      <c r="G14">
-        <v>1.26</v>
-      </c>
-      <c r="H14">
-        <v>1.28</v>
-      </c>
-      <c r="I14" t="s">
-        <v>141</v>
-      </c>
-      <c r="J14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15">
-        <v>1.05</v>
-      </c>
-      <c r="E15">
-        <v>1.05</v>
-      </c>
-      <c r="F15">
-        <v>1.05</v>
-      </c>
-      <c r="G15">
-        <v>1.05</v>
-      </c>
-      <c r="H15">
-        <v>1.05</v>
-      </c>
-      <c r="I15" t="s">
-        <v>141</v>
-      </c>
-      <c r="J15" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16">
-        <v>1.2</v>
-      </c>
-      <c r="E16">
-        <v>1.2</v>
-      </c>
-      <c r="F16">
-        <v>1.2</v>
-      </c>
-      <c r="G16">
-        <v>1.2</v>
-      </c>
-      <c r="H16">
-        <v>1.2</v>
-      </c>
-      <c r="J16" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="J17" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>192</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="F18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H18">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J18" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19">
-        <v>1.2</v>
-      </c>
-      <c r="E19">
-        <v>1.18</v>
-      </c>
-      <c r="F19">
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="G19">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="H19">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J19" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20">
-        <v>2</v>
-      </c>
-      <c r="E20">
-        <v>1.8</v>
-      </c>
-      <c r="F20">
-        <v>1.6</v>
-      </c>
-      <c r="G20">
-        <v>1.4</v>
-      </c>
-      <c r="H20">
-        <v>1.25</v>
-      </c>
-      <c r="J20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21">
-        <v>1.05</v>
-      </c>
-      <c r="E21">
-        <v>1.06</v>
-      </c>
-      <c r="F21">
-        <v>1.07</v>
-      </c>
-      <c r="G21">
-        <v>1.08</v>
-      </c>
-      <c r="H21">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="J21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D2:H2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A26ADBE-5182-4739-A39F-809BE890F4A3}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2020</v>
-      </c>
-      <c r="B2" s="8">
-        <v>5.44E-4</v>
-      </c>
-      <c r="C2" s="8">
-        <v>5.44E-4</v>
-      </c>
-      <c r="D2" s="8">
-        <v>5.44E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2025</v>
-      </c>
-      <c r="B3" s="8">
-        <v>1.2720000000000001E-3</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1.7719999999999999E-3</v>
-      </c>
-      <c r="D3" s="8">
-        <v>5.44E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2030</v>
-      </c>
-      <c r="B4" s="8">
-        <v>2E-3</v>
-      </c>
-      <c r="C4" s="8">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="D4" s="8">
-        <v>5.44E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2040</v>
-      </c>
-      <c r="B5" s="8">
-        <v>3.4559999999999999E-3</v>
-      </c>
-      <c r="C5" s="8">
-        <v>5.4559999999999999E-3</v>
-      </c>
-      <c r="D5" s="8">
-        <v>5.44E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2050</v>
-      </c>
-      <c r="B6" s="8">
-        <v>4.9120000000000006E-3</v>
-      </c>
-      <c r="C6" s="8">
-        <v>7.9119999999999989E-3</v>
-      </c>
-      <c r="D6" s="8">
-        <v>5.44E-4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BE84BF-E76A-402B-AF31-6F26AF2044C4}">
-  <dimension ref="A1:A22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="144.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>221</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96CB461-6F71-44E3-A168-71729D7C3877}">
-  <dimension ref="A1:C49"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="116.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>184</v>
-      </c>
-      <c r="B12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>158</v>
-      </c>
-      <c r="B13" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>182</v>
-      </c>
-      <c r="B14" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>185</v>
-      </c>
-      <c r="B15" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>183</v>
-      </c>
-      <c r="B21" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A21" r:id="rId1" xr:uid="{6BB6211E-19A0-4F02-BC7A-3A56508CA64B}"/>
-    <hyperlink ref="A19" r:id="rId2" xr:uid="{E125BC90-7F30-4B94-A86A-3EFCF7E2E423}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD9D518-1F19-4A80-A28B-711CA74E3278}">
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="116.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>196</v>
-      </c>
-      <c r="B4" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B5" t="s">
-        <v>199</v>
-      </c>
-      <c r="C5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>200</v>
-      </c>
-      <c r="B7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>204</v>
-      </c>
-      <c r="B8" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>209</v>
-      </c>
-      <c r="B14" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" t="s">
-        <v>156</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A14" r:id="rId1" xr:uid="{C4319978-B66A-4039-B91C-E1EE64F3642A}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EE6192-3357-4DF0-8055-1C716AB42B8C}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29715,12 +30380,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D42CA7-36D4-4300-B367-C77E8D5E25CA}">
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B21" sqref="A3:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30030,7 +30695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B08A794-8873-43D6-A027-1749091B636F}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -30293,7 +30958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA07C27-4DA3-4DC0-BE20-62D49702D364}">
   <dimension ref="A1:Z58"/>
   <sheetViews>
@@ -33485,7 +34150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CDBB70-C564-430C-8368-0301BECC4495}">
   <dimension ref="A1:O25"/>
   <sheetViews>
@@ -34156,7 +34821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DA41B5-4555-4ECC-9A08-B1A926FD14EC}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
@@ -35057,7 +35722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C003461F-E7F2-4532-B47B-B811710E9E75}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -35091,266 +35756,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4663A21-150A-4914-BC6D-954E6813A5C4}">
-  <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to new fleet renewal setup
</commit_message>
<xml_diff>
--- a/Data/transport_costs_emissions_raw.xlsx
+++ b/Data/transport_costs_emissions_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50135F56-8232-48B0-89C8-A3BAA42E8A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{50135F56-8232-48B0-89C8-A3BAA42E8A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C0D241-7438-45D8-B187-40E116F6F7CF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{5AE32870-AF16-462E-B631-817A89F76936}"/>
+    <workbookView xWindow="13800" yWindow="0" windowWidth="30345" windowHeight="23400" firstSheet="2" activeTab="10" xr2:uid="{5AE32870-AF16-462E-B631-817A89F76936}"/>
   </bookViews>
   <sheets>
     <sheet name="LEGEND" sheetId="27" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3349" uniqueCount="243">
   <si>
     <t>Mode</t>
   </si>
@@ -822,10 +822,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1068,7 +1068,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="39">
@@ -1077,9 +1077,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1100,12 +1100,12 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -1421,7 +1421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1432,7 +1432,7 @@
   <dimension ref="B1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1811,223 +1811,43 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9569D7EE-B770-468F-B61A-E0DB82253C9A}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
+      <c r="B2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>192</v>
-      </c>
-      <c r="C16">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19">
+      <c r="B4">
         <v>30</v>
       </c>
     </row>
@@ -34845,7 +34665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DA41B5-4555-4ECC-9A08-B1A926FD14EC}">
   <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
log and temp folder required
</commit_message>
<xml_diff>
--- a/Data/transport_costs_emissions_raw.xlsx
+++ b/Data/transport_costs_emissions_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{50135F56-8232-48B0-89C8-A3BAA42E8A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BF43A45-696B-4319-8ECE-2BD88CA97F74}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{50135F56-8232-48B0-89C8-A3BAA42E8A84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD639988-B6B9-484A-9BFB-D777A2719D55}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="60" windowWidth="13515" windowHeight="23190" firstSheet="2" activeTab="2" xr2:uid="{5AE32870-AF16-462E-B631-817A89F76936}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" firstSheet="2" activeTab="13" xr2:uid="{5AE32870-AF16-462E-B631-817A89F76936}"/>
   </bookViews>
   <sheets>
     <sheet name="LEGEND" sheetId="27" r:id="rId1"/>
@@ -1077,7 +1077,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1086,9 +1086,9 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -1109,9 +1109,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -1138,8 +1137,913 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="nb-NO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CO2_fee!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CO2_fee!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.44E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2720000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4559999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9120000000000006E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-32D1-4EE3-92F8-0720F7F89071}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="750805384"/>
+        <c:axId val="750804304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="750805384"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="750804304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="750804304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="750805384"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nb-NO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{485E06EA-447F-0910-D1F6-B3D682C8BA88}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1431,7 +2335,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1525,12 +2429,12 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="36" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2061,13 +2965,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -2648,8 +3552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A26ADBE-5182-4739-A39F-809BE890F4A3}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,6 +3650,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2768,7 +3673,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2808,7 +3713,7 @@
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="34" t="s">
         <v>165</v>
       </c>
     </row>
@@ -2885,7 +3790,7 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="34" t="s">
         <v>169</v>
       </c>
     </row>
@@ -2938,7 +3843,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="34" t="s">
         <v>159</v>
       </c>
     </row>
@@ -2976,7 +3881,7 @@
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="34" t="s">
         <v>160</v>
       </c>
     </row>
@@ -3119,7 +4024,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="34" t="s">
         <v>169</v>
       </c>
     </row>
@@ -3175,7 +4080,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+      <c r="A10" s="34" t="s">
         <v>159</v>
       </c>
     </row>
@@ -3188,7 +4093,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="34" t="s">
         <v>160</v>
       </c>
     </row>
@@ -29963,8 +30868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EE6192-3357-4DF0-8055-1C716AB42B8C}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29999,10 +30904,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4">
@@ -30013,10 +30918,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5">
@@ -30024,10 +30929,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6">
@@ -30035,45 +30940,32 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7">
         <f>(127+217)/2</f>
         <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8">
         <v>156</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="31"/>
-      <c r="C9" s="31"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="C10" s="31"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C11" s="31"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="C12" s="31"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -30120,7 +31012,7 @@
         <f>(42/14000)*9000</f>
         <v>27</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="35" t="s">
         <v>217</v>
       </c>
     </row>
@@ -30138,7 +31030,7 @@
         <f>(28/4000)*2500</f>
         <v>17.5</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="35" t="s">
         <v>217</v>
       </c>
     </row>
@@ -30156,7 +31048,7 @@
         <f>(12/15000)*17000</f>
         <v>13.600000000000001</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="35" t="s">
         <v>217</v>
       </c>
     </row>
@@ -34033,7 +34925,6 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
       <c r="B3" s="1" t="s">
         <v>125</v>
       </c>
@@ -34045,10 +34936,6 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
       <c r="M3" s="1" t="s">
         <v>125</v>
       </c>
@@ -34056,7 +34943,6 @@
       <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="31"/>
       <c r="B4" s="1" t="s">
         <v>126</v>
       </c>
@@ -34078,10 +34964,6 @@
       <c r="H4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
       <c r="M4" s="1" t="s">
         <v>126</v>
       </c>
@@ -34096,40 +34978,37 @@
       <c r="A5" s="1">
         <v>2022</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <v>1.2767928712592653</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="31">
         <v>2.1213845775913618</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="31">
         <v>2.1937387804084145</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <v>70.025688013948354</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="31">
         <v>9999999</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="31">
         <v>9999999</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="31">
         <v>232.0320116775589</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
       <c r="L5" s="1">
         <v>2022</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="31">
         <v>7.0669961483799351E-2</v>
       </c>
-      <c r="O5" s="32">
+      <c r="O5" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
     </row>
@@ -34137,40 +35016,37 @@
       <c r="A6" s="1">
         <v>2026</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <v>1.2763128712592651</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <v>1.8539131909777176</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <v>1.8635831400519962</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <v>69.950946714649291</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="31">
         <v>9999999</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="31">
         <v>9999999</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="31">
         <v>180.62313348765065</v>
       </c>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
       <c r="L6" s="1">
         <v>2026</v>
       </c>
-      <c r="M6" s="32">
+      <c r="M6" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="N6" s="32">
+      <c r="N6" s="31">
         <v>6.42564725061298E-2</v>
       </c>
-      <c r="O6" s="32">
+      <c r="O6" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
     </row>
@@ -34178,40 +35054,37 @@
       <c r="A7" s="1">
         <v>2030</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="31">
         <v>1.2759928712592652</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>1.6422220976950082</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <v>1.6846665595885915</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <v>69.901119181783244</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="31">
         <v>151.86171664778865</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="31">
         <v>146.84521118705186</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="31">
         <v>152.76384663352172</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
       <c r="L7" s="1">
         <v>2030</v>
       </c>
-      <c r="M7" s="32">
+      <c r="M7" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="N7" s="32">
+      <c r="N7" s="31">
         <v>4.8759740450291647E-2</v>
       </c>
-      <c r="O7" s="32">
+      <c r="O7" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
     </row>
@@ -34219,40 +35092,37 @@
       <c r="A8" s="1">
         <v>2035</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="31">
         <v>1.2757528712592652</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>1.4955046571342974</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>1.587752224593614</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <v>69.863748532133712</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="31">
         <v>137.06926759396413</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <v>134.23510106777977</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="31">
         <v>137.67321472054223</v>
       </c>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
       <c r="L8" s="1">
         <v>2035</v>
       </c>
-      <c r="M8" s="32">
+      <c r="M8" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="N8" s="32">
+      <c r="N8" s="31">
         <v>3.5837105494588684E-2</v>
       </c>
-      <c r="O8" s="32">
+      <c r="O8" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
     </row>
@@ -34260,40 +35130,37 @@
       <c r="A9" s="1">
         <v>2040</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="31">
         <v>1.2755528712592652</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="31">
         <v>1.4378216218112176</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>1.5271776831432882</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <v>69.832606324092424</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="31">
         <v>123.02464296908737</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="31">
         <v>121.70752317473068</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="31">
         <v>128.24108986128627</v>
       </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
       <c r="L9" s="1">
         <v>2040</v>
       </c>
-      <c r="M9" s="32">
+      <c r="M9" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="N9" s="32">
+      <c r="N9" s="31">
         <v>2.5030000097816377E-2</v>
       </c>
-      <c r="O9" s="32">
+      <c r="O9" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
     </row>
@@ -34301,40 +35168,37 @@
       <c r="A10" s="1">
         <v>2045</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>1.2753688712592655</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>1.4011312462807095</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <v>1.4827240084814306</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <v>69.803955492694442</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="31">
         <v>111.25576902822024</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <v>109.46912942997312</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <v>121.31916193869151</v>
       </c>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
       <c r="L10" s="1">
         <v>2045</v>
       </c>
-      <c r="M10" s="32">
+      <c r="M10" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="N10" s="32">
+      <c r="N10" s="31">
         <v>2.3516659509040184E-2</v>
       </c>
-      <c r="O10" s="32">
+      <c r="O10" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
     </row>
@@ -34342,59 +35206,53 @@
       <c r="A11" s="1">
         <v>2050</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="31">
         <v>1.2751928712592653</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="31">
         <v>1.3759969700023786</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="31">
         <v>1.4462779141014377</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="31">
         <v>69.77655034961812</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="31">
         <v>100.95840459329722</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="31">
         <v>98.429822230140488</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="31">
         <v>115.64410267132213</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
       <c r="L11" s="1">
         <v>2050</v>
       </c>
-      <c r="M11" s="32">
+      <c r="M11" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="N11" s="32">
+      <c r="N11" s="31">
         <v>2.2340826533588171E-2</v>
       </c>
-      <c r="O11" s="32">
+      <c r="O11" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32"/>
-      <c r="O12" s="32"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -34405,7 +35263,6 @@
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
       <c r="B17" s="1" t="s">
         <v>125</v>
       </c>
@@ -34419,7 +35276,6 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
       <c r="B18" s="1" t="s">
         <v>126</v>
       </c>
@@ -34446,31 +35302,31 @@
       <c r="A19" s="1">
         <v>2022</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="31">
         <f>B5-M5</f>
         <v>1.2590620565500683</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <f t="shared" ref="C19:D25" si="0">C5-N5</f>
         <v>2.0507146161075624</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="31">
         <f t="shared" si="0"/>
         <v>2.1760079656992177</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <f>E5</f>
         <v>70.025688013948354</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="31">
         <f t="shared" ref="F19:H19" si="1">F5</f>
         <v>9999999</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="31">
         <f t="shared" si="1"/>
         <v>9999999</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="31">
         <f t="shared" si="1"/>
         <v>232.0320116775589</v>
       </c>
@@ -34479,31 +35335,31 @@
       <c r="A20" s="1">
         <v>2026</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="31">
         <f t="shared" ref="B20:B25" si="2">B6-M6</f>
         <v>1.2585820565500681</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <f t="shared" si="0"/>
         <v>1.7896567184715877</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="31">
         <f t="shared" si="0"/>
         <v>1.8458523253427992</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="31">
         <f t="shared" ref="E20:H25" si="3">E6</f>
         <v>69.950946714649291</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="31">
         <f t="shared" si="3"/>
         <v>9999999</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="31">
         <f t="shared" si="3"/>
         <v>9999999</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="31">
         <f t="shared" si="3"/>
         <v>180.62313348765065</v>
       </c>
@@ -34512,31 +35368,31 @@
       <c r="A21" s="1">
         <v>2030</v>
       </c>
-      <c r="B21" s="32">
+      <c r="B21" s="31">
         <f t="shared" si="2"/>
         <v>1.2582620565500682</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <f t="shared" si="0"/>
         <v>1.5934623572447164</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="31">
         <f t="shared" si="0"/>
         <v>1.6669357448793944</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="31">
         <f t="shared" si="3"/>
         <v>69.901119181783244</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="31">
         <f t="shared" si="3"/>
         <v>151.86171664778865</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="31">
         <f t="shared" si="3"/>
         <v>146.84521118705186</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="31">
         <f t="shared" si="3"/>
         <v>152.76384663352172</v>
       </c>
@@ -34545,31 +35401,31 @@
       <c r="A22" s="1">
         <v>2035</v>
       </c>
-      <c r="B22" s="32">
+      <c r="B22" s="31">
         <f t="shared" si="2"/>
         <v>1.2580220565500682</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <f t="shared" si="0"/>
         <v>1.4596675516397086</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="31">
         <f t="shared" si="0"/>
         <v>1.570021409884417</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="31">
         <f t="shared" si="3"/>
         <v>69.863748532133712</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="31">
         <f t="shared" si="3"/>
         <v>137.06926759396413</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="31">
         <f t="shared" si="3"/>
         <v>134.23510106777977</v>
       </c>
-      <c r="H22" s="32">
+      <c r="H22" s="31">
         <f t="shared" si="3"/>
         <v>137.67321472054223</v>
       </c>
@@ -34578,31 +35434,31 @@
       <c r="A23" s="1">
         <v>2040</v>
       </c>
-      <c r="B23" s="32">
+      <c r="B23" s="31">
         <f t="shared" si="2"/>
         <v>1.2578220565500682</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="31">
         <f t="shared" si="0"/>
         <v>1.4127916217134013</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="31">
         <f t="shared" si="0"/>
         <v>1.5094468684340911</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="31">
         <f t="shared" si="3"/>
         <v>69.832606324092424</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="31">
         <f t="shared" si="3"/>
         <v>123.02464296908737</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="31">
         <f t="shared" si="3"/>
         <v>121.70752317473068</v>
       </c>
-      <c r="H23" s="32">
+      <c r="H23" s="31">
         <f t="shared" si="3"/>
         <v>128.24108986128627</v>
       </c>
@@ -34611,31 +35467,31 @@
       <c r="A24" s="1">
         <v>2045</v>
       </c>
-      <c r="B24" s="32">
+      <c r="B24" s="31">
         <f t="shared" si="2"/>
         <v>1.2576380565500684</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="31">
         <f t="shared" si="0"/>
         <v>1.3776145867716694</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="31">
         <f t="shared" si="0"/>
         <v>1.4649931937722336</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="31">
         <f t="shared" si="3"/>
         <v>69.803955492694442</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="31">
         <f t="shared" si="3"/>
         <v>111.25576902822024</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="31">
         <f t="shared" si="3"/>
         <v>109.46912942997312</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="31">
         <f t="shared" si="3"/>
         <v>121.31916193869151</v>
       </c>
@@ -34644,31 +35500,31 @@
       <c r="A25" s="1">
         <v>2050</v>
       </c>
-      <c r="B25" s="32">
+      <c r="B25" s="31">
         <f t="shared" si="2"/>
         <v>1.2574620565500683</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="31">
         <f t="shared" si="0"/>
         <v>1.3536561434687904</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="31">
         <f t="shared" si="0"/>
         <v>1.4285470993922407</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="31">
         <f t="shared" si="3"/>
         <v>69.77655034961812</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="31">
         <f t="shared" si="3"/>
         <v>100.95840459329722</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="31">
         <f t="shared" si="3"/>
         <v>98.429822230140488</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="31">
         <f t="shared" si="3"/>
         <v>115.64410267132213</v>
       </c>
@@ -34703,8 +35559,6 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
       <c r="C3" s="1">
         <v>2022</v>
       </c>
@@ -34726,8 +35580,6 @@
       <c r="I3" s="1">
         <v>2050</v>
       </c>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
       <c r="N3" s="1">
         <v>2022</v>
       </c>
@@ -34757,25 +35609,25 @@
       <c r="B4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="31">
         <v>1.2767928712592653</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="31">
         <v>1.2763128712592651</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="31">
         <v>1.2759928712592652</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="31">
         <v>1.2757528712592652</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="31">
         <v>1.2755528712592652</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="31">
         <v>1.2753688712592655</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="31">
         <v>1.2751928712592653</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -34784,25 +35636,25 @@
       <c r="M4" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="N4" s="32">
+      <c r="N4" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="O4" s="32">
+      <c r="O4" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="P4" s="32">
+      <c r="P4" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="Q4" s="32">
+      <c r="Q4" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="R4" s="32">
+      <c r="R4" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="S4" s="32">
+      <c r="S4" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="T4" s="32">
+      <c r="T4" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
     </row>
@@ -34811,50 +35663,50 @@
       <c r="B5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="31">
         <v>2.1213845775913618</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="31">
         <v>1.8539131909777176</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="31">
         <v>1.6422220976950082</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="31">
         <v>1.4955046571342974</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="31">
         <v>1.4378216218112176</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="31">
         <v>1.4011312462807095</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="31">
         <v>1.3759969700023786</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="31">
         <v>7.0669961483799351E-2</v>
       </c>
-      <c r="O5" s="32">
+      <c r="O5" s="31">
         <v>6.42564725061298E-2</v>
       </c>
-      <c r="P5" s="32">
+      <c r="P5" s="31">
         <v>4.8759740450291647E-2</v>
       </c>
-      <c r="Q5" s="32">
+      <c r="Q5" s="31">
         <v>3.5837105494588684E-2</v>
       </c>
-      <c r="R5" s="32">
+      <c r="R5" s="31">
         <v>2.5030000097816377E-2</v>
       </c>
-      <c r="S5" s="32">
+      <c r="S5" s="31">
         <v>2.3516659509040184E-2</v>
       </c>
-      <c r="T5" s="32">
+      <c r="T5" s="31">
         <v>2.2340826533588171E-2</v>
       </c>
     </row>
@@ -34863,50 +35715,50 @@
       <c r="B6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="31">
         <v>2.1937387804084145</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="31">
         <v>1.8635831400519962</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="31">
         <v>1.6846665595885915</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="31">
         <v>1.587752224593614</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="31">
         <v>1.5271776831432882</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="31">
         <v>1.4827240084814306</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="31">
         <v>1.4462779141014377</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="N6" s="32">
+      <c r="N6" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="O6" s="32">
+      <c r="O6" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="P6" s="32">
+      <c r="P6" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="Q6" s="32">
+      <c r="Q6" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="R6" s="32">
+      <c r="R6" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="S6" s="32">
+      <c r="S6" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
-      <c r="T6" s="32">
+      <c r="T6" s="31">
         <v>1.7730814709196963E-2</v>
       </c>
     </row>
@@ -34917,130 +35769,130 @@
       <c r="B7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <v>70.025688013948354</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="31">
         <v>69.950946714649291</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="31">
         <v>69.901119181783244</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="31">
         <v>69.863748532133712</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="31">
         <v>69.832606324092424</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="31">
         <v>69.803955492694442</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="31">
         <v>69.77655034961812</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>999999</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="31">
         <v>999999</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="31">
         <v>151.86171664778865</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="31">
         <v>137.06926759396413</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="31">
         <v>123.02464296908737</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="31">
         <v>111.25576902822024</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="31">
         <v>100.95840459329722</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="31">
         <v>999999</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>999999</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="31">
         <v>146.84521118705186</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="31">
         <v>134.23510106777977</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="31">
         <v>121.70752317473068</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="31">
         <v>109.46912942997312</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="31">
         <v>98.429822230140488</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>232.0320116775589</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="31">
         <v>180.62313348765065</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="31">
         <v>152.76384663352172</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="31">
         <v>137.67321472054223</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="31">
         <v>128.24108986128627</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="31">
         <v>121.31916193869151</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="31">
         <v>115.64410267132213</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L11" s="1"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -35080,73 +35932,73 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="31">
         <f t="shared" ref="C16:I18" si="0">C4-N4</f>
         <v>1.2590620565500683</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="31">
         <f t="shared" si="0"/>
         <v>1.2585820565500681</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="31">
         <f t="shared" si="0"/>
         <v>1.2582620565500682</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="31">
         <f t="shared" si="0"/>
         <v>1.2580220565500682</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="31">
         <f t="shared" si="0"/>
         <v>1.2578220565500682</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="31">
         <f t="shared" si="0"/>
         <v>1.2576380565500684</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="31">
         <f t="shared" si="0"/>
         <v>1.2574620565500683</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="31">
         <f t="shared" si="0"/>
         <v>2.0507146161075624</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="31">
         <f t="shared" si="0"/>
         <v>1.7896567184715877</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="31">
         <f t="shared" si="0"/>
         <v>1.5934623572447164</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="31">
         <f t="shared" si="0"/>
         <v>1.4596675516397086</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="31">
         <f t="shared" si="0"/>
         <v>1.4127916217134013</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="31">
         <f t="shared" si="0"/>
         <v>1.3776145867716694</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="31">
         <f t="shared" si="0"/>
         <v>1.3536561434687904</v>
       </c>
@@ -35161,44 +36013,43 @@
       <c r="AB17" s="1"/>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" t="s">
         <v>128</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="31">
         <f t="shared" si="0"/>
         <v>2.1760079656992177</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="31">
         <f t="shared" si="0"/>
         <v>1.8458523253427992</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="31">
         <f t="shared" si="0"/>
         <v>1.6669357448793944</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="31">
         <f t="shared" si="0"/>
         <v>1.570021409884417</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="31">
         <f t="shared" si="0"/>
         <v>1.5094468684340911</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="31">
         <f t="shared" si="0"/>
         <v>1.4649931937722336</v>
       </c>
-      <c r="I18" s="32">
+      <c r="I18" s="31">
         <f t="shared" si="0"/>
         <v>1.4285470993922407</v>
       </c>
       <c r="K18" t="s">
         <v>145</v>
       </c>
-      <c r="Q18" s="31"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -35212,41 +36063,40 @@
       <c r="AB18" s="1"/>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <f t="shared" ref="C19:I22" si="1">C7</f>
         <v>70.025688013948354</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="31">
         <f t="shared" si="1"/>
         <v>69.950946714649291</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="31">
         <f t="shared" si="1"/>
         <v>69.901119181783244</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="31">
         <f t="shared" si="1"/>
         <v>69.863748532133712</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="31">
         <f t="shared" si="1"/>
         <v>69.832606324092424</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="31">
         <f t="shared" si="1"/>
         <v>69.803955492694442</v>
       </c>
-      <c r="I19" s="32">
+      <c r="I19" s="31">
         <f t="shared" si="1"/>
         <v>69.77655034961812</v>
       </c>
-      <c r="Q19" s="31"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
@@ -35260,43 +36110,43 @@
       <c r="AB19" s="1"/>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <f t="shared" si="1"/>
         <v>999999</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="31">
         <f t="shared" si="1"/>
         <v>999999</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="31">
         <f t="shared" si="1"/>
         <v>151.86171664778865</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="31">
         <f t="shared" si="1"/>
         <v>137.06926759396413</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="31">
         <f t="shared" si="1"/>
         <v>123.02464296908737</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="31">
         <f t="shared" si="1"/>
         <v>111.25576902822024</v>
       </c>
-      <c r="I20" s="32">
+      <c r="I20" s="31">
         <f t="shared" si="1"/>
         <v>100.95840459329722</v>
       </c>
       <c r="Q20" s="1"/>
-      <c r="R20" s="32"/>
-      <c r="S20" s="32"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="31"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -35308,43 +36158,43 @@
       <c r="AB20" s="1"/>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <f t="shared" si="1"/>
         <v>999999</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="31">
         <f t="shared" si="1"/>
         <v>999999</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="31">
         <f t="shared" si="1"/>
         <v>146.84521118705186</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="31">
         <f t="shared" si="1"/>
         <v>134.23510106777977</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="31">
         <f t="shared" si="1"/>
         <v>121.70752317473068</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="31">
         <f t="shared" si="1"/>
         <v>109.46912942997312</v>
       </c>
-      <c r="I21" s="32">
+      <c r="I21" s="31">
         <f t="shared" si="1"/>
         <v>98.429822230140488</v>
       </c>
       <c r="Q21" s="1"/>
-      <c r="R21" s="32"/>
-      <c r="S21" s="32"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
@@ -35356,37 +36206,37 @@
       <c r="AB21" s="1"/>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <f t="shared" si="1"/>
         <v>232.0320116775589</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="31">
         <f t="shared" si="1"/>
         <v>180.62313348765065</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="31">
         <f t="shared" si="1"/>
         <v>152.76384663352172</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="31">
         <f t="shared" si="1"/>
         <v>137.67321472054223</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="31">
         <f t="shared" si="1"/>
         <v>128.24108986128627</v>
       </c>
-      <c r="H22" s="32">
+      <c r="H22" s="31">
         <f t="shared" si="1"/>
         <v>121.31916193869151</v>
       </c>
-      <c r="I22" s="32">
+      <c r="I22" s="31">
         <f t="shared" si="1"/>
         <v>115.64410267132213</v>
       </c>
@@ -35394,8 +36244,8 @@
         <v>146</v>
       </c>
       <c r="Q22" s="1"/>
-      <c r="R22" s="32"/>
-      <c r="S22" s="32"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
@@ -35407,11 +36257,9 @@
       <c r="AB22" s="1"/>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
-      <c r="B23" s="31"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="32"/>
-      <c r="S23" s="32"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="31"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
@@ -35423,16 +36271,16 @@
       <c r="AB23" s="1"/>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="32"/>
-      <c r="S24" s="32"/>
+      <c r="R24" s="31"/>
+      <c r="S24" s="31"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
@@ -35448,8 +36296,8 @@
         <v>191</v>
       </c>
       <c r="Q25" s="1"/>
-      <c r="R25" s="32"/>
-      <c r="S25" s="32"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
@@ -35462,8 +36310,8 @@
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q26" s="1"/>
-      <c r="R26" s="32"/>
-      <c r="S26" s="32"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="31"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
@@ -35488,8 +36336,8 @@
         <v>190</v>
       </c>
       <c r="Q27" s="1"/>
-      <c r="R27" s="32"/>
-      <c r="S27" s="32"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
@@ -35524,7 +36372,7 @@
       <c r="AB28" s="1"/>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" t="s">
         <v>32</v>
       </c>
       <c r="B29" t="s">
@@ -35561,7 +36409,7 @@
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31" t="s">
@@ -35606,7 +36454,7 @@
       <c r="A2">
         <v>9.6300000000000008</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="33">
         <v>44650</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update of Vehicle Types
</commit_message>
<xml_diff>
--- a/Data/transport_costs_emissions_raw.xlsx
+++ b/Data/transport_costs_emissions_raw.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/STraM_ntnu_development/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{54B285D2-970E-4AFE-A7E1-52E969457EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C6F85BB1-6D07-4114-8903-3066592611FA}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{54B285D2-970E-4AFE-A7E1-52E969457EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A65C804C-7FAF-4465-809A-033E18FA16A7}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="6590" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{5AE32870-AF16-462E-B631-817A89F76936}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="28800" windowHeight="22170" firstSheet="2" activeTab="9" xr2:uid="{5AE32870-AF16-462E-B631-817A89F76936}"/>
   </bookViews>
   <sheets>
     <sheet name="LEGEND" sheetId="27" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3355" uniqueCount="251">
   <si>
     <t>Mode</t>
   </si>
@@ -816,6 +816,30 @@
   <si>
     <t>From</t>
   </si>
+  <si>
+    <t>Break bulk</t>
+  </si>
+  <si>
+    <t>Container</t>
+  </si>
+  <si>
+    <t>Liquid bulk</t>
+  </si>
+  <si>
+    <t>System trains (Liquid bulk)</t>
+  </si>
+  <si>
+    <t>Neo bulk</t>
+  </si>
+  <si>
+    <t>Neo bulk truck with hanger</t>
+  </si>
+  <si>
+    <t>Neo bulk trains</t>
+  </si>
+  <si>
+    <t>Product class</t>
+  </si>
 </sst>
 </file>
 
@@ -1071,7 +1095,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1112,7 +1136,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2458,9 +2481,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4663A21-150A-4914-BC6D-954E6813A5C4}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2473,7 +2498,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>250</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -2495,7 +2520,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>244</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -2506,10 +2531,10 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>243</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2517,10 +2542,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>247</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2528,32 +2553,32 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>244</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2561,10 +2586,10 @@
         <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>243</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2572,10 +2597,10 @@
         <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>247</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2583,54 +2608,54 @@
         <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>245</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>244</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>243</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>247</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -2638,76 +2663,10 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>245</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -31428,7 +31387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B08A794-8873-43D6-A027-1749091B636F}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -31471,10 +31430,10 @@
       <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="16">
@@ -31513,10 +31472,10 @@
       <c r="A6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="16">
@@ -31555,10 +31514,10 @@
       <c r="A9" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="16">
@@ -31597,10 +31556,10 @@
       <c r="A12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="16">
@@ -31639,10 +31598,10 @@
       <c r="A15" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="16">
@@ -31681,10 +31640,10 @@
       <c r="A18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="16">
@@ -31723,10 +31682,10 @@
       <c r="A21" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" t="s">
         <v>6</v>
       </c>
       <c r="D21" s="16">

</xml_diff>